<commit_message>
map working with application
</commit_message>
<xml_diff>
--- a/covid.xlsx
+++ b/covid.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Area</t>
   </si>
@@ -23,9 +23,6 @@
   </si>
   <si>
     <t>New York City, NY</t>
-  </si>
-  <si>
-    <t>positive</t>
   </si>
 </sst>
 </file>
@@ -375,8 +372,8 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
+      <c r="B2">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>